<commit_message>
AutoLoan Customer Search feature
</commit_message>
<xml_diff>
--- a/Gowtham_ULS_New/TestData/IjaraJSPaths.xlsx
+++ b/Gowtham_ULS_New/TestData/IjaraJSPaths.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" firstSheet="19" activeTab="23"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ijara_loginElements" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="1777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="1779">
   <si>
     <t>Ijara_LoginFieldName</t>
   </si>
@@ -5368,6 +5368,12 @@
   </si>
   <si>
     <t>StatusField</t>
+  </si>
+  <si>
+    <t>PleaseFillToastPopUp</t>
+  </si>
+  <si>
+    <t>document.querySelector('div[id="toast-container"] button+div')</t>
   </si>
 </sst>
 </file>
@@ -10050,7 +10056,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12402,8 +12408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13340,8 +13346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14188,8 +14194,12 @@
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="7"/>
-      <c r="B108" s="7"/>
+      <c r="A108" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1778</v>
+      </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="7"/>

</xml_diff>

<commit_message>
Persoanl Loan feature test cases Commit
</commit_message>
<xml_diff>
--- a/Gowtham_ULS_New/TestData/IjaraJSPaths.xlsx
+++ b/Gowtham_ULS_New/TestData/IjaraJSPaths.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540" firstSheet="20" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Ijara_loginElements" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,14 @@
     <sheet name="MurApDataEntryAppDetails" sheetId="24" r:id="rId22"/>
     <sheet name="MuADCheckLivingExpenses" sheetId="25" r:id="rId23"/>
     <sheet name="MuADCheckRepaymentMode" sheetId="26" r:id="rId24"/>
+    <sheet name="PLNewAppCustomerDetails" sheetId="27" r:id="rId25"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="1779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="1979">
   <si>
     <t>Ijara_LoginFieldName</t>
   </si>
@@ -5374,6 +5375,606 @@
   </si>
   <si>
     <t>document.querySelector('div[id="toast-container"] button+div')</t>
+  </si>
+  <si>
+    <t>customer_details_tab</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-segment-button[id="seg2"]')</t>
+  </si>
+  <si>
+    <t>customerDetails_AddButton</t>
+  </si>
+  <si>
+    <t>application_type_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="SCR.APPLICANT.TYPE.TOOLTIP"]+ion-select')</t>
+  </si>
+  <si>
+    <t>customer_details_type_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="CUSTOMERDETAILS_CUSTOMER_TYPE."]+ion-select')</t>
+  </si>
+  <si>
+    <t>title_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="CUSTOMERDETAILSISLAMIC_SALUTAT"]+ion-select')</t>
+  </si>
+  <si>
+    <t>first_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerFirstName"] input')</t>
+  </si>
+  <si>
+    <t>first_Name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerFirstName"] ion-label').innerText</t>
+  </si>
+  <si>
+    <t>middle_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerMiddleName"] input')</t>
+  </si>
+  <si>
+    <t>middle_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerMiddleName"] ion-label').innerText</t>
+  </si>
+  <si>
+    <t>last_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerLastName"] input')</t>
+  </si>
+  <si>
+    <t>last_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerLastName"] ion-label').innerText</t>
+  </si>
+  <si>
+    <t>family_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerThirdName"] input')</t>
+  </si>
+  <si>
+    <t>family_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerThirdName"] ion-label').innerText</t>
+  </si>
+  <si>
+    <t>first_name_arabic_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerFirstNameInOtherLang"] input')</t>
+  </si>
+  <si>
+    <t>first_name_arabic_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerFirstNameInOtherLang"] ion-label').innerText</t>
+  </si>
+  <si>
+    <t>middle_name_arabic_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerMiddleNameInOtherLang"] input')</t>
+  </si>
+  <si>
+    <t>middle_name_arabic_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerMiddleNameInOtherLang"] ion-label').innerText</t>
+  </si>
+  <si>
+    <t>last_name_arabic_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerLastNameInOtherLang"] input')</t>
+  </si>
+  <si>
+    <t>last_name_arabic_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerLastNameInOtherLang"] ion-label').innerText</t>
+  </si>
+  <si>
+    <t>family_name_arabic_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerNameInOtherLang"] input')</t>
+  </si>
+  <si>
+    <t>family_name_arabic_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerNameInOtherLang"] ion-label').innerText</t>
+  </si>
+  <si>
+    <t>date_of_birth_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-prime-date[ng-reflect-title="LEAD_DETAILS.DOB"] input')</t>
+  </si>
+  <si>
+    <t>date_of_birth_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-prime-date[ng-reflect-title="LEAD_DETAILS.DOB"]').innerText</t>
+  </si>
+  <si>
+    <t>date_of_birth_field_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-prime-date[ng-reflect-title="LEAD_DETAILS.DOB"] p-calendar').getAttribute('ng-reflect-date-format')</t>
+  </si>
+  <si>
+    <t>age_input_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.AGE.TOOLTIP"]+ion-input input').getAttribute('type')</t>
+  </si>
+  <si>
+    <t>age_get_value</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.AGE.TOOLTIP"]+ion-input input').value</t>
+  </si>
+  <si>
+    <t>age_field_editable_check</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.AGE.TOOLTIP"]+ion-input').getAttribute('ng-reflect-readonly')</t>
+  </si>
+  <si>
+    <t>age_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.AGE.TOOLTIP"]').innerText</t>
+  </si>
+  <si>
+    <t>gender_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="SCR.GENDER.TOOLTIP"]+ion-select')</t>
+  </si>
+  <si>
+    <t>maritail_status_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.MARITAL_STATUS.TO"]+ion-select')</t>
+  </si>
+  <si>
+    <t>education_level_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.EDUCATION_LEVEL.T"]+ion-select')</t>
+  </si>
+  <si>
+    <t>nationality_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.NATIONALITY.TOOLT"]+ion-select')</t>
+  </si>
+  <si>
+    <t>customer_residential_status_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="CUSTOMERDETAILS_RESIDENTIAL_ST"]+ion-select')</t>
+  </si>
+  <si>
+    <t>languages_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.LANGUAGE.TOOLTIP"]+ion-select')</t>
+  </si>
+  <si>
+    <t>client_category_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[ng-reflect-name="clientCategory"] ion-select')</t>
+  </si>
+  <si>
+    <t>consent_obtained_for_credit_bureau_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="Consent Obtained for Credit Bu"]+ion-select')</t>
+  </si>
+  <si>
+    <t>no_of_dependents_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.NO_OF_DEPENDENTS."]+ion-input input')</t>
+  </si>
+  <si>
+    <t>no_of_dependents_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.NO_OF_DEPENDENTS."]').innerText</t>
+  </si>
+  <si>
+    <t>remarks_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="remarks"] ion-input input')</t>
+  </si>
+  <si>
+    <t>remarks_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="remarks"] ion-label').innerText</t>
+  </si>
+  <si>
+    <t>status_toggle_button</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-radio-button[id="recStatus"] ion-toggle')</t>
+  </si>
+  <si>
+    <t>get_record_status</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-radio-button[id="recStatus"] ion-toggle').getAttribute('aria-checked')</t>
+  </si>
+  <si>
+    <t>list_view_record_status</t>
+  </si>
+  <si>
+    <t>document.querySelector('td[ng-reflect-ng-switch="badge"] span&gt;span').innerText</t>
+  </si>
+  <si>
+    <t>blacklisted_toggle</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-radio-button[ng-reflect-title="SCR.BLACKLISTED"] ion-toggle')</t>
+  </si>
+  <si>
+    <t>blacklisted_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="Blacklisted"]').innerText</t>
+  </si>
+  <si>
+    <t>date_highlighted_button</t>
+  </si>
+  <si>
+    <t>document.querySelector('span[tabindex="0"]')</t>
+  </si>
+  <si>
+    <t>first_name_input_field_level_validation</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="customerFirstName"]+div ion-badge').innerText</t>
+  </si>
+  <si>
+    <t>customer_details_list_view_edit_button</t>
+  </si>
+  <si>
+    <t>customer_details_list_view_first_name</t>
+  </si>
+  <si>
+    <t>document.querySelector('td[ng-reflect-ng-switch="string"] p-celleditor[class="p-element ng-star-inserted"] span').innerText</t>
+  </si>
+  <si>
+    <t>customer_details_list_view_search_result</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-grid p-paginator[ng-reflect-rows="5"] span[class="p-paginator-current ng-star-inserted"]').innerText</t>
+  </si>
+  <si>
+    <t>customer_details_list_view_search_button</t>
+  </si>
+  <si>
+    <t>document.querySelector('button[icon="pi pi-search"]')</t>
+  </si>
+  <si>
+    <t>customer_details_list_view_search_input</t>
+  </si>
+  <si>
+    <t>customer_details_export_button</t>
+  </si>
+  <si>
+    <t>document.querySelector('p-dropdown[placeholder="Export"] span[class$= "p-placeholder ng-star-inserted"]')</t>
+  </si>
+  <si>
+    <t>customer_details_excel_export_option</t>
+  </si>
+  <si>
+    <t>customer_details_pdf_export_option</t>
+  </si>
+  <si>
+    <t>customer_details_back_button_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-title[class$="ion-color-dark md title-default hydrated"]').innerText</t>
+  </si>
+  <si>
+    <t>customer_details_list_view_record</t>
+  </si>
+  <si>
+    <t>document.querySelector('p-table[ng-reflect-data-key="id"] thead[class="p-datatable-thead"]').innerText</t>
+  </si>
+  <si>
+    <t>document.querySelector('tbody td[ng-reflect-ng-switch="string"]')</t>
+  </si>
+  <si>
+    <t>no_of_childer_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnNum1"] input')</t>
+  </si>
+  <si>
+    <t>no_of_children_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnNum1"]').innerText</t>
+  </si>
+  <si>
+    <t>salutation_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="salutation"] ion-select')</t>
+  </si>
+  <si>
+    <t>salutation_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="salutation"]').innerText</t>
+  </si>
+  <si>
+    <t>father_first_name_Input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar1"] input')</t>
+  </si>
+  <si>
+    <t>father_first_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar1"]').innerText</t>
+  </si>
+  <si>
+    <t>father_middle_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar2"] input')</t>
+  </si>
+  <si>
+    <t>father_middle_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar2"]').innerText</t>
+  </si>
+  <si>
+    <t>father_last_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar3"] input')</t>
+  </si>
+  <si>
+    <t>father_last_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar3"]').innerText</t>
+  </si>
+  <si>
+    <t>spouse_first_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar4"] input')</t>
+  </si>
+  <si>
+    <t>spouse_first_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar4"]').innerText</t>
+  </si>
+  <si>
+    <t>spouse_middle_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar5"] input')</t>
+  </si>
+  <si>
+    <t>spouse_middle_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar5"]').innerText</t>
+  </si>
+  <si>
+    <t>spouse_last_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar6"] input')</t>
+  </si>
+  <si>
+    <t>spouse_last_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="extnChar6"]').innerText</t>
+  </si>
+  <si>
+    <t>spouse_status_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="dynamicNumericField1"] ion-select')</t>
+  </si>
+  <si>
+    <t>spouse_status_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="dynamicNumericField1"]').innerText</t>
+  </si>
+  <si>
+    <t>gender_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="SCR.GENDER.TOOLTIP"]').innerText</t>
+  </si>
+  <si>
+    <t>maritail_status_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.MARITAL_STATUS.TO"]').innerText</t>
+  </si>
+  <si>
+    <t>educational_level_mandatory_verificatiion</t>
+  </si>
+  <si>
+    <t>document.querySelector('ion-label[ng-reflect-text="LEAD_DETAILS.EDUCATION_LEVEL.T"]').innerText</t>
+  </si>
+  <si>
+    <t>category_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="ethnicType"] ion-select')</t>
+  </si>
+  <si>
+    <t>relegion_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="religion"] ion-select')</t>
+  </si>
+  <si>
+    <t>mothers_maiden_name_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="mothersName"] input')</t>
+  </si>
+  <si>
+    <t>mothers_maiden_name_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="mothersName"]').innerText</t>
+  </si>
+  <si>
+    <t>type_of_residency_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="residenceType"] ion-select')</t>
+  </si>
+  <si>
+    <t>industry_segmentation_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="clientCategory"] ion-select')</t>
+  </si>
+  <si>
+    <t>is_income_considered_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="isIncomeConsidered"] ion-select')</t>
+  </si>
+  <si>
+    <t>customer_profile_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="dynamicCharField1"] ion-select')</t>
+  </si>
+  <si>
+    <t>relationship_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="relationship"] ion-select')</t>
+  </si>
+  <si>
+    <t>isPoliticallyExposed_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="isPoliticallyExposed"] ion-select')</t>
+  </si>
+  <si>
+    <t>remarks_field_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="remarks"] textarea')</t>
+  </si>
+  <si>
+    <t>remarks_field_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="remarks"]').innerText</t>
+  </si>
+  <si>
+    <t>existing_customer_flag</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-radio-button[id="existingCustomerFlag"] ion-toggle')</t>
+  </si>
+  <si>
+    <t>existing_customer_flag_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-radio-button[id="existingCustomerFlag"]').innerText</t>
+  </si>
+  <si>
+    <t>is_blacklisted_flg</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-radio-button[id="isBlacklisted"] ion-toggle')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="phone1"] input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="phone1"]').innerText</t>
+  </si>
+  <si>
+    <t>mobile1_number_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="mobile1"] input')</t>
+  </si>
+  <si>
+    <t>mobileNumber_primary_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="mobile1"]').innerText</t>
+  </si>
+  <si>
+    <t>mobile_number_secondary_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="mobile2"] input')</t>
+  </si>
+  <si>
+    <t>mobile_number_secondory_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="mobile2"]').innerText</t>
+  </si>
+  <si>
+    <t>email_input</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="email"] input')</t>
+  </si>
+  <si>
+    <t>email_mandatory_verification</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="email"]').innerText</t>
+  </si>
+  <si>
+    <t>prefered_contact_method_dropdown</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-select-layout[id="preferredContactMethod"] ion-select')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="preferredContactTime"] input')</t>
+  </si>
+  <si>
+    <t>document.querySelector('digital-text-box[id="preferredContactTime"]').innerText</t>
   </si>
 </sst>
 </file>
@@ -12049,9 +12650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12599,6 +13198,881 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>1864</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B49" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>1873</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B53" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>1931</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>1933</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>1943</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>1947</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>1957</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>1963</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>1965</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B107" t="s">
+        <v>762</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B28"/>
@@ -13346,7 +14820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>

</xml_diff>